<commit_message>
SCR - Planilha - Ajuste na senha
</commit_message>
<xml_diff>
--- a/resource/inputs/SCR_INTERAGINDO_COM_PLANILHA.xlsx
+++ b/resource/inputs/SCR_INTERAGINDO_COM_PLANILHA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\CursoRobot\RobotFramework\ExemplosEstruturas\resource\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DC0ADBA-FEA0-48CA-B0B1-CAA3D8B166EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2483A30-5292-4BB0-8146-D8F974CA91E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{99ED8967-220D-4B7D-ABBC-2E58C5458409}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{99ED8967-220D-4B7D-ABBC-2E58C5458409}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Ambiente</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>dayvsontp@hotmail.com</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>28092019</t>
   </si>
 </sst>
 </file>
@@ -169,11 +175,11 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -489,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B2F53D-474B-44EC-A21C-009F916860EE}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,26 +508,29 @@
     <col min="3" max="3" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>28092019</v>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>